<commit_message>
Added Repeated DNA Sequences
</commit_message>
<xml_diff>
--- a/Leetcode.xlsx
+++ b/Leetcode.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="645">
   <si>
     <t>LeetCode Problem Statistics</t>
   </si>
@@ -30718,6 +30718,166 @@
         <rFont val="Helvetica"/>
       </rPr>
       <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">Repeated DNA Sequences </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Easiest way can be store those substrings in a set. But how to further reduce the space usage? The key is that storing string is too much. Design a hash function to map substrings to a key that won’t collide.  +Observing that A=0x41, C=0x43, G=0x47, T=0x54, the last 3 bits of them are different. 10 * 3 = 30 bits &lt; 32, which can be represented use an int. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>1. Use integer as key, boolean as value to build a map +    Map&lt;Integer, Boolean&gt; map = new HashMap&lt;Integer, Boolean&gt;(); +2. Traverse the string +    for (int t = 0, i = 0; i &lt; s.length(); i++) +3. Move bit mask left 3 bits, and with 30 1s, and set last 3 bits with current char +    t = (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>t &lt;&lt; 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve"> &amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>0x3FFFFFFF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">) | (s.charAt(i) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>&amp; 7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">); +4. Check key in map, if yes, get the value, if true, add to result, set to false +    if (map.containsKey(t)) {
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">        if (map.get(t)) {
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">            res.add(s.substring(i - 9, i + 1));
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">            map.put(t, false); // false means already added
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">        }
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">    } +5. If not in map, put in map +    else { 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">        map.put(t, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="10"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">); // true means showed up but not added
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">    }</t>
     </r>
   </si>
   <si>
@@ -36665,7 +36825,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:I15"/>
+  <dimension ref="A2:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozenSplit"/>
@@ -37052,6 +37212,35 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
+    <row r="16" ht="212.35" customHeight="1">
+      <c r="A16" s="4">
+        <v>187</v>
+      </c>
+      <c r="B16" t="s" s="5">
+        <v>628</v>
+      </c>
+      <c r="C16" t="s" s="4">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s" s="5">
+        <v>476</v>
+      </c>
+      <c r="E16" t="s" s="5">
+        <v>629</v>
+      </c>
+      <c r="F16" t="s" s="5">
+        <v>630</v>
+      </c>
+      <c r="G16" t="s" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s" s="4">
+        <v>320</v>
+      </c>
+      <c r="I16" t="s" s="4">
+        <v>320</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
@@ -37069,6 +37258,7 @@
     <hyperlink ref="B12" r:id="rId10" location="" tooltip="" display=""/>
     <hyperlink ref="B13" r:id="rId11" location="" tooltip="" display=""/>
     <hyperlink ref="B15" r:id="rId12" location="" tooltip="" display=""/>
+    <hyperlink ref="B16" r:id="rId13" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -37137,7 +37327,7 @@
         <v>156</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="C2" t="s" s="4">
         <v>17</v>
@@ -37146,7 +37336,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" t="s" s="4">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="13"/>
@@ -37156,7 +37346,7 @@
         <v>157</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="C3" t="s" s="4">
         <v>47</v>
@@ -37165,7 +37355,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" t="s" s="4">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="13"/>
@@ -37175,7 +37365,7 @@
         <v>158</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="C4" t="s" s="4">
         <v>11</v>
@@ -37184,7 +37374,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" t="s" s="4">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="H4" s="6"/>
       <c r="I4" s="13"/>
@@ -37194,7 +37384,7 @@
         <v>159</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="C5" t="s" s="4">
         <v>11</v>
@@ -37203,7 +37393,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" t="s" s="4">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="13"/>
@@ -37213,7 +37403,7 @@
         <v>159</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="C6" t="s" s="4">
         <v>11</v>
@@ -37222,7 +37412,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" t="s" s="4">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="13"/>
@@ -37232,7 +37422,7 @@
         <v>161</v>
       </c>
       <c r="B7" t="s" s="5">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="C7" t="s" s="4">
         <v>17</v>
@@ -37241,7 +37431,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" t="s" s="4">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="13"/>
@@ -37251,7 +37441,7 @@
         <v>163</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="C8" t="s" s="4">
         <v>17</v>
@@ -37260,7 +37450,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" t="s" s="4">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="13"/>
@@ -37270,7 +37460,7 @@
         <v>167</v>
       </c>
       <c r="B9" t="s" s="5">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="C9" t="s" s="4">
         <v>17</v>
@@ -37279,7 +37469,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" t="s" s="4">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="16"/>
@@ -37289,7 +37479,7 @@
         <v>170</v>
       </c>
       <c r="B10" t="s" s="5">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="C10" t="s" s="4">
         <v>47</v>
@@ -37298,7 +37488,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" t="s" s="4">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="13"/>
@@ -37348,23 +37538,23 @@
         <v>2</v>
       </c>
       <c r="C2" t="s" s="3">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="3" ht="152.55" customHeight="1">
       <c r="B3" t="s" s="10">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>639</v>
+        <v>642</v>
       </c>
     </row>
     <row r="4" ht="92.35" customHeight="1">
       <c r="B4" t="s" s="10">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="C4" t="s" s="5">
-        <v>641</v>
+        <v>644</v>
       </c>
     </row>
     <row r="5" ht="20.35" customHeight="1">

</xml_diff>